<commit_message>
completed dHAP4 input sheet (questions remain)
</commit_message>
<xml_diff>
--- a/data/GRNmap_input_workbooks/15-genes_28-edges_BK-dHAP4-fam_no-strains-added_Sigmoid_estimation.xlsx
+++ b/data/GRNmap_input_workbooks/15-genes_28-edges_BK-dHAP4-fam_no-strains-added_Sigmoid_estimation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10300" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="-80" yWindow="0" windowWidth="23140" windowHeight="15540" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="production_rates" sheetId="5" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="38">
   <si>
     <t>ACE2</t>
   </si>
@@ -87,13 +87,67 @@
   <si>
     <t>threshold_b</t>
   </si>
+  <si>
+    <t>alpha</t>
+  </si>
+  <si>
+    <t>kk_max</t>
+  </si>
+  <si>
+    <t>MaxIter</t>
+  </si>
+  <si>
+    <t>TolFun</t>
+  </si>
+  <si>
+    <t>MaxFunEval</t>
+  </si>
+  <si>
+    <t>TolX</t>
+  </si>
+  <si>
+    <t>production_function</t>
+  </si>
+  <si>
+    <t>L_curve</t>
+  </si>
+  <si>
+    <t>estimate_params</t>
+  </si>
+  <si>
+    <t>make_graphs</t>
+  </si>
+  <si>
+    <t>fix_P</t>
+  </si>
+  <si>
+    <t>fix_b</t>
+  </si>
+  <si>
+    <t>expression_timepoints</t>
+  </si>
+  <si>
+    <t>Strain</t>
+  </si>
+  <si>
+    <t>simulation_timepoints</t>
+  </si>
+  <si>
+    <t>Sigmoid</t>
+  </si>
+  <si>
+    <t>wt</t>
+  </si>
+  <si>
+    <t>dhap4</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -152,7 +206,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="151">
+  <cellStyleXfs count="235">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -304,15 +358,103 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="151">
+  <cellStyles count="235">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -388,6 +530,48 @@
     <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -463,6 +647,48 @@
     <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -816,15 +1042,17 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="14.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="12" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>16</v>
       </c>
@@ -832,7 +1060,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" ht="12" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -840,7 +1068,7 @@
         <v>-0.22359586469675655</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" ht="12" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -848,7 +1076,7 @@
         <v>-0.43321698784996576</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" ht="12" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -856,7 +1084,7 @@
         <v>-0.2009122262492595</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" ht="12" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -864,7 +1092,7 @@
         <v>-0.19254088348887369</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" ht="12" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -872,7 +1100,7 @@
         <v>-0.32239403746974199</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" ht="12" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -880,7 +1108,7 @@
         <v>-0.27182242374899818</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" ht="12" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -888,7 +1116,7 @@
         <v>-9.9021025794277892E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" ht="12" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -896,7 +1124,7 @@
         <v>-0.40773363562349724</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" ht="12" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -904,7 +1132,7 @@
         <v>-0.69314718055994529</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" ht="12" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -912,7 +1140,7 @@
         <v>-0.14002973344645359</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" ht="12" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -920,7 +1148,7 @@
         <v>-0.28291721655507968</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" ht="12" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -928,7 +1156,7 @@
         <v>-0.32239403746974199</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" ht="12" customHeight="1">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -936,7 +1164,7 @@
         <v>-0.17328679513998632</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" ht="12" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -944,7 +1172,7 @@
         <v>-0.72962861111573196</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" ht="12" customHeight="1">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -968,12 +1196,14 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A1:B16"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="15.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1117,15 +1347,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X17"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X22" sqref="X22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="16384" width="10.83203125" style="2"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:14" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>16</v>
       </c>
@@ -1168,38 +1401,8 @@
       <c r="N1" s="1">
         <v>60</v>
       </c>
-      <c r="O1" s="1">
-        <v>90</v>
-      </c>
-      <c r="P1" s="1">
-        <v>90</v>
-      </c>
-      <c r="Q1" s="1">
-        <v>90</v>
-      </c>
-      <c r="R1" s="1">
-        <v>90</v>
-      </c>
-      <c r="S1" s="1">
-        <v>90</v>
-      </c>
-      <c r="T1" s="1">
-        <v>120</v>
-      </c>
-      <c r="U1" s="1">
-        <v>120</v>
-      </c>
-      <c r="V1" s="1">
-        <v>120</v>
-      </c>
-      <c r="W1" s="1">
-        <v>120</v>
-      </c>
-      <c r="X1" s="1">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24">
+    </row>
+    <row r="2" spans="1:14" s="2" customFormat="1">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1242,38 +1445,8 @@
       <c r="N2" s="1">
         <v>-1.2497</v>
       </c>
-      <c r="O2" s="1">
-        <v>4.1700000000000001E-2</v>
-      </c>
-      <c r="P2" s="4">
-        <v>-0.38429999999999997</v>
-      </c>
-      <c r="Q2" s="1">
-        <v>0.26819999999999999</v>
-      </c>
-      <c r="R2" s="1">
-        <v>-0.64459999999999995</v>
-      </c>
-      <c r="S2" s="1">
-        <v>-1.2023999999999999</v>
-      </c>
-      <c r="T2" s="1">
-        <v>1.2668999999999999</v>
-      </c>
-      <c r="U2" s="1">
-        <v>0.66649999999999998</v>
-      </c>
-      <c r="V2" s="1">
-        <v>1.0752999999999999</v>
-      </c>
-      <c r="W2" s="1">
-        <v>-0.33379999999999999</v>
-      </c>
-      <c r="X2" s="1">
-        <v>-0.31900000000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24">
+    </row>
+    <row r="3" spans="1:14" s="2" customFormat="1">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1316,38 +1489,8 @@
       <c r="N3" s="1">
         <v>-0.92479999999999996</v>
       </c>
-      <c r="O3" s="1">
-        <v>0.65269999999999995</v>
-      </c>
-      <c r="P3" s="1">
-        <v>2.1187999999999998</v>
-      </c>
-      <c r="Q3" s="1">
-        <v>0.23130000000000001</v>
-      </c>
-      <c r="R3" s="1">
-        <v>1.2464</v>
-      </c>
-      <c r="S3" s="1">
-        <v>-0.57269999999999999</v>
-      </c>
-      <c r="T3" s="1">
-        <v>-2.1888999999999998</v>
-      </c>
-      <c r="U3" s="1">
-        <v>0.12939999999999999</v>
-      </c>
-      <c r="V3" s="1">
-        <v>-2.7945000000000002</v>
-      </c>
-      <c r="W3" s="1">
-        <v>-0.37840000000000001</v>
-      </c>
-      <c r="X3" s="1">
-        <v>5.2900000000000003E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24">
+    </row>
+    <row r="4" spans="1:14" s="2" customFormat="1">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -1390,38 +1533,8 @@
       <c r="N4" s="1">
         <v>1.4784999999999999</v>
       </c>
-      <c r="O4" s="1">
-        <v>0.89829999999999999</v>
-      </c>
-      <c r="P4" s="1">
-        <v>-2.0207999999999999</v>
-      </c>
-      <c r="Q4" s="1">
-        <v>-1.4488000000000001</v>
-      </c>
-      <c r="R4" s="1">
-        <v>-1.72E-2</v>
-      </c>
-      <c r="S4" s="1">
-        <v>0.5534</v>
-      </c>
-      <c r="T4" s="1">
-        <v>3.3799999999999997E-2</v>
-      </c>
-      <c r="U4" s="1">
-        <v>-0.7984</v>
-      </c>
-      <c r="V4" s="1">
-        <v>-2.1122000000000001</v>
-      </c>
-      <c r="W4" s="1">
-        <v>-5.74E-2</v>
-      </c>
-      <c r="X4" s="1">
-        <v>1.0625</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24">
+    </row>
+    <row r="5" spans="1:14" s="2" customFormat="1">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -1464,38 +1577,8 @@
       <c r="N5" s="1">
         <v>-0.35849999999999999</v>
       </c>
-      <c r="O5" s="1">
-        <v>-0.52</v>
-      </c>
-      <c r="P5" s="1">
-        <v>3.6999999999999998E-2</v>
-      </c>
-      <c r="Q5" s="1">
-        <v>-0.19520000000000001</v>
-      </c>
-      <c r="R5" s="1">
-        <v>-0.62109999999999999</v>
-      </c>
-      <c r="S5" s="1">
-        <v>1.0991</v>
-      </c>
-      <c r="T5" s="1">
-        <v>-1.1580999999999999</v>
-      </c>
-      <c r="U5" s="1">
-        <v>-0.15840000000000001</v>
-      </c>
-      <c r="V5" s="1">
-        <v>-2.9499999999999998E-2</v>
-      </c>
-      <c r="W5" s="1">
-        <v>-0.44340000000000002</v>
-      </c>
-      <c r="X5" s="1">
-        <v>-1.1623000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24">
+    </row>
+    <row r="6" spans="1:14" s="2" customFormat="1">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -1538,38 +1621,8 @@
       <c r="N6" s="1">
         <v>0.1953</v>
       </c>
-      <c r="O6" s="1">
-        <v>0.63180000000000003</v>
-      </c>
-      <c r="P6" s="1">
-        <v>-0.49559999999999998</v>
-      </c>
-      <c r="Q6" s="1">
-        <v>1.1919999999999999</v>
-      </c>
-      <c r="R6" s="1">
-        <v>-0.38900000000000001</v>
-      </c>
-      <c r="S6" s="1">
-        <v>-0.92969999999999997</v>
-      </c>
-      <c r="T6" s="1">
-        <v>0.29210000000000003</v>
-      </c>
-      <c r="U6" s="1">
-        <v>-0.63919999999999999</v>
-      </c>
-      <c r="V6" s="1">
-        <v>-3.1608000000000001</v>
-      </c>
-      <c r="W6" s="1">
-        <v>0.42</v>
-      </c>
-      <c r="X6" s="1">
-        <v>-1.4531000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24">
+    </row>
+    <row r="7" spans="1:14" s="2" customFormat="1">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -1612,38 +1665,8 @@
       <c r="N7" s="1">
         <v>-1.8463000000000001</v>
       </c>
-      <c r="O7" s="1">
-        <v>-3.0074999999999998</v>
-      </c>
-      <c r="P7" s="1">
-        <v>-0.85760000000000003</v>
-      </c>
-      <c r="Q7" s="1">
-        <v>0.20369999999999999</v>
-      </c>
-      <c r="R7" s="1">
-        <v>0.1341</v>
-      </c>
-      <c r="S7" s="1">
-        <v>-0.1076</v>
-      </c>
-      <c r="T7" s="1">
-        <v>-0.4667</v>
-      </c>
-      <c r="U7" s="1">
-        <v>-1.8031999999999999</v>
-      </c>
-      <c r="V7" s="1">
-        <v>0.81240000000000001</v>
-      </c>
-      <c r="W7" s="1">
-        <v>-4.4200000000000003E-2</v>
-      </c>
-      <c r="X7" s="1">
-        <v>-1.0219</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24">
+    </row>
+    <row r="8" spans="1:14" s="2" customFormat="1">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -1686,38 +1709,8 @@
       <c r="N8" s="1">
         <v>2.2172000000000001</v>
       </c>
-      <c r="O8" s="1">
-        <v>2.2862</v>
-      </c>
-      <c r="P8" s="1">
-        <v>-0.81799999999999995</v>
-      </c>
-      <c r="Q8" s="1">
-        <v>0.48199999999999998</v>
-      </c>
-      <c r="R8" s="1">
-        <v>0.32540000000000002</v>
-      </c>
-      <c r="S8" s="1">
-        <v>0.74180000000000001</v>
-      </c>
-      <c r="T8" s="1">
-        <v>0.45</v>
-      </c>
-      <c r="U8" s="1">
-        <v>-0.26840000000000003</v>
-      </c>
-      <c r="V8" s="1">
-        <v>-2.1374</v>
-      </c>
-      <c r="W8" s="1">
-        <v>-0.63129999999999997</v>
-      </c>
-      <c r="X8" s="1">
-        <v>0.7853</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24">
+    </row>
+    <row r="9" spans="1:14" s="2" customFormat="1">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -1760,38 +1753,8 @@
       <c r="N9" s="1">
         <v>-0.12709999999999999</v>
       </c>
-      <c r="O9" s="1">
-        <v>0.8175</v>
-      </c>
-      <c r="P9" s="1">
-        <v>-0.12620000000000001</v>
-      </c>
-      <c r="Q9" s="1">
-        <v>0.24429999999999999</v>
-      </c>
-      <c r="R9" s="1">
-        <v>0.94</v>
-      </c>
-      <c r="S9" s="1">
-        <v>-6.3500000000000001E-2</v>
-      </c>
-      <c r="T9" s="1">
-        <v>1.0230999999999999</v>
-      </c>
-      <c r="U9" s="1">
-        <v>0.43459999999999999</v>
-      </c>
-      <c r="V9" s="1">
-        <v>0.1696</v>
-      </c>
-      <c r="W9" s="1">
-        <v>-0.64080000000000004</v>
-      </c>
-      <c r="X9" s="1">
-        <v>0.47389999999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24">
+    </row>
+    <row r="10" spans="1:14" s="2" customFormat="1">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -1834,38 +1797,8 @@
       <c r="N10" s="1">
         <v>-1.0367</v>
       </c>
-      <c r="O10" s="1">
-        <v>-0.13200000000000001</v>
-      </c>
-      <c r="P10" s="1">
-        <v>-1.4322999999999999</v>
-      </c>
-      <c r="Q10" s="1">
-        <v>-0.48180000000000001</v>
-      </c>
-      <c r="R10" s="1">
-        <v>0.5786</v>
-      </c>
-      <c r="S10" s="1">
-        <v>0.49509999999999998</v>
-      </c>
-      <c r="T10" s="1">
-        <v>-0.49419999999999997</v>
-      </c>
-      <c r="U10" s="1">
-        <v>-0.94699999999999995</v>
-      </c>
-      <c r="V10" s="1">
-        <v>-1.1869000000000001</v>
-      </c>
-      <c r="W10" s="1">
-        <v>4.9500000000000002E-2</v>
-      </c>
-      <c r="X10" s="1">
-        <v>0.40789999999999998</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24">
+    </row>
+    <row r="11" spans="1:14" s="2" customFormat="1">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -1908,38 +1841,8 @@
       <c r="N11" s="1">
         <v>-0.27479999999999999</v>
       </c>
-      <c r="O11" s="1">
-        <v>0.33600000000000002</v>
-      </c>
-      <c r="P11" s="1">
-        <v>-1.0723</v>
-      </c>
-      <c r="Q11" s="1">
-        <v>0.38729999999999998</v>
-      </c>
-      <c r="R11" s="1">
-        <v>0.12180000000000001</v>
-      </c>
-      <c r="S11" s="1">
-        <v>-0.44950000000000001</v>
-      </c>
-      <c r="T11" s="1">
-        <v>0.65210000000000001</v>
-      </c>
-      <c r="U11" s="1">
-        <v>-0.94159999999999999</v>
-      </c>
-      <c r="V11" s="1">
-        <v>-0.51380000000000003</v>
-      </c>
-      <c r="W11" s="1">
-        <v>-0.1426</v>
-      </c>
-      <c r="X11" s="1">
-        <v>-0.47739999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24">
+    </row>
+    <row r="12" spans="1:14" s="2" customFormat="1">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -1982,38 +1885,8 @@
       <c r="N12" s="1">
         <v>0.28120000000000001</v>
       </c>
-      <c r="O12" s="1">
-        <v>-0.36559999999999998</v>
-      </c>
-      <c r="P12" s="1">
-        <v>-5.7599999999999998E-2</v>
-      </c>
-      <c r="Q12" s="1">
-        <v>1.1876</v>
-      </c>
-      <c r="R12" s="1">
-        <v>0.31469999999999998</v>
-      </c>
-      <c r="S12" s="1">
-        <v>-0.70920000000000005</v>
-      </c>
-      <c r="T12" s="1">
-        <v>-1.1857</v>
-      </c>
-      <c r="U12" s="1">
-        <v>-1.0833999999999999</v>
-      </c>
-      <c r="V12" s="1">
-        <v>1.6509</v>
-      </c>
-      <c r="W12" s="1">
-        <v>-0.9194</v>
-      </c>
-      <c r="X12" s="1">
-        <v>-0.95709999999999995</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24">
+    </row>
+    <row r="13" spans="1:14" s="2" customFormat="1">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -2056,38 +1929,8 @@
       <c r="N13" s="1">
         <v>9.7000000000000003E-2</v>
       </c>
-      <c r="O13" s="1">
-        <v>0.1263</v>
-      </c>
-      <c r="P13" s="1">
-        <v>0.20549999999999999</v>
-      </c>
-      <c r="Q13" s="1">
-        <v>-0.7208</v>
-      </c>
-      <c r="R13" s="1">
-        <v>-0.70430000000000004</v>
-      </c>
-      <c r="S13" s="1">
-        <v>-0.16120000000000001</v>
-      </c>
-      <c r="T13" s="1">
-        <v>0.27560000000000001</v>
-      </c>
-      <c r="U13" s="1">
-        <v>1.1964999999999999</v>
-      </c>
-      <c r="V13" s="1">
-        <v>0.2424</v>
-      </c>
-      <c r="W13" s="1">
-        <v>0.6603</v>
-      </c>
-      <c r="X13" s="1">
-        <v>0.51490000000000002</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24">
+    </row>
+    <row r="14" spans="1:14" s="2" customFormat="1">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -2130,38 +1973,8 @@
       <c r="N14" s="1">
         <v>-0.72499999999999998</v>
       </c>
-      <c r="O14" s="1">
-        <v>0.5837</v>
-      </c>
-      <c r="P14" s="1">
-        <v>0.61250000000000004</v>
-      </c>
-      <c r="Q14" s="1">
-        <v>-0.46800000000000003</v>
-      </c>
-      <c r="R14" s="1">
-        <v>-0.56240000000000001</v>
-      </c>
-      <c r="S14" s="1">
-        <v>0.55410000000000004</v>
-      </c>
-      <c r="T14" s="1">
-        <v>0.82450000000000001</v>
-      </c>
-      <c r="U14" s="1">
-        <v>1.177</v>
-      </c>
-      <c r="V14" s="1">
-        <v>1.1002000000000001</v>
-      </c>
-      <c r="W14" s="1">
-        <v>0.65090000000000003</v>
-      </c>
-      <c r="X14" s="4">
-        <v>0.93820000000000003</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24">
+    </row>
+    <row r="15" spans="1:14" s="2" customFormat="1">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -2204,38 +2017,8 @@
       <c r="N15" s="1">
         <v>-0.51170000000000004</v>
       </c>
-      <c r="O15" s="1">
-        <v>2.2915000000000001</v>
-      </c>
-      <c r="P15" s="1">
-        <v>0.85609999999999997</v>
-      </c>
-      <c r="Q15" s="1">
-        <v>2.7856999999999998</v>
-      </c>
-      <c r="R15" s="1">
-        <v>2.0832000000000002</v>
-      </c>
-      <c r="S15" s="1">
-        <v>1.1548</v>
-      </c>
-      <c r="T15" s="1">
-        <v>-0.28310000000000002</v>
-      </c>
-      <c r="U15" s="1">
-        <v>-0.47220000000000001</v>
-      </c>
-      <c r="V15" s="1">
-        <v>0.15240000000000001</v>
-      </c>
-      <c r="W15" s="1">
-        <v>1.2243999999999999</v>
-      </c>
-      <c r="X15" s="1">
-        <v>-1.379</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24">
+    </row>
+    <row r="16" spans="1:14" s="2" customFormat="1">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -2278,69 +2061,11 @@
       <c r="N16" s="4">
         <v>2.6345999999999998</v>
       </c>
-      <c r="O16" s="1">
-        <v>0.45350000000000001</v>
-      </c>
-      <c r="P16" s="1">
-        <v>9.4399999999999998E-2</v>
-      </c>
-      <c r="Q16" s="1">
-        <v>-1.4200000000000001E-2</v>
-      </c>
-      <c r="R16" s="1">
-        <v>1.6395</v>
-      </c>
-      <c r="S16" s="1">
-        <v>-0.27450000000000002</v>
-      </c>
-      <c r="T16" s="1">
-        <v>0.35289999999999999</v>
-      </c>
-      <c r="U16" s="1">
-        <v>-1.0243</v>
-      </c>
-      <c r="V16" s="1">
-        <v>-0.77610000000000001</v>
-      </c>
-      <c r="W16" s="1">
-        <v>0.83430000000000004</v>
-      </c>
-      <c r="X16" s="1">
-        <v>0.52370000000000005</v>
-      </c>
-    </row>
-    <row r="17" spans="1:24">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+    </row>
+    <row r="17" spans="7:7" s="2" customFormat="1">
       <c r="G17" s="3"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
-      <c r="Q17" s="2"/>
-      <c r="R17" s="2"/>
-      <c r="S17" s="2"/>
-      <c r="T17" s="2"/>
-      <c r="U17" s="2"/>
-      <c r="V17" s="2"/>
-      <c r="W17" s="2"/>
-      <c r="X17" s="2"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:X16">
-    <cfRule type="containsBlanks" dxfId="1" priority="1">
-      <formula>LEN(TRIM(B1))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -2353,15 +2078,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X17"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="16384" width="10.83203125" style="2"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:14" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>16</v>
       </c>
@@ -2390,7 +2118,7 @@
         <v>30</v>
       </c>
       <c r="J1" s="1">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="K1" s="1">
         <v>60</v>
@@ -2401,147 +2129,627 @@
       <c r="M1" s="1">
         <v>60</v>
       </c>
-      <c r="N1" s="1">
-        <v>60</v>
-      </c>
-      <c r="O1" s="1">
-        <v>90</v>
-      </c>
-      <c r="P1" s="1">
-        <v>90</v>
-      </c>
-      <c r="Q1" s="1">
-        <v>90</v>
-      </c>
-      <c r="R1" s="1">
-        <v>90</v>
-      </c>
-      <c r="S1" s="1">
-        <v>90</v>
-      </c>
-      <c r="T1" s="1">
-        <v>120</v>
-      </c>
-      <c r="U1" s="1">
-        <v>120</v>
-      </c>
-      <c r="V1" s="1">
-        <v>120</v>
-      </c>
-      <c r="W1" s="1">
-        <v>120</v>
-      </c>
-      <c r="X1" s="1">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24">
+      <c r="N1" s="1"/>
+    </row>
+    <row r="2" spans="1:14" s="2" customFormat="1">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:24">
+      <c r="B2" s="2">
+        <v>-0.55800000000000005</v>
+      </c>
+      <c r="C2" s="2">
+        <v>-0.313</v>
+      </c>
+      <c r="D2" s="2">
+        <v>-8.8599999999999998E-2</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.56740000000000002</v>
+      </c>
+      <c r="F2" s="2">
+        <v>-0.44800000000000001</v>
+      </c>
+      <c r="G2" s="2">
+        <v>-0.4768</v>
+      </c>
+      <c r="H2" s="2">
+        <v>-0.59799999999999998</v>
+      </c>
+      <c r="I2" s="2">
+        <v>-0.1176</v>
+      </c>
+      <c r="J2" s="2">
+        <v>-0.27829999999999999</v>
+      </c>
+      <c r="K2" s="2">
+        <v>-0.60829999999999995</v>
+      </c>
+      <c r="L2" s="2">
+        <v>-0.6331</v>
+      </c>
+      <c r="M2" s="2">
+        <v>0.19850000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="2" customFormat="1">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:24">
+      <c r="B3" s="2">
+        <v>-1.5401</v>
+      </c>
+      <c r="C3" s="2">
+        <v>-5.2299999999999999E-2</v>
+      </c>
+      <c r="D3" s="2">
+        <v>-0.7026</v>
+      </c>
+      <c r="E3" s="2">
+        <v>-0.49330000000000002</v>
+      </c>
+      <c r="F3" s="2">
+        <v>-0.81669999999999998</v>
+      </c>
+      <c r="G3" s="2">
+        <v>-2.8E-3</v>
+      </c>
+      <c r="H3" s="2">
+        <v>-0.65680000000000005</v>
+      </c>
+      <c r="I3" s="2">
+        <v>-1.0266999999999999</v>
+      </c>
+      <c r="J3" s="2">
+        <v>-1.9866999999999999</v>
+      </c>
+      <c r="K3" s="2">
+        <v>-1.5253000000000001</v>
+      </c>
+      <c r="L3" s="2">
+        <v>-1.0837000000000001</v>
+      </c>
+      <c r="M3" s="2">
+        <v>-1.5982000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" s="2" customFormat="1">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:24">
+      <c r="B4" s="2">
+        <v>-0.39429999999999998</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3.0979999999999999</v>
+      </c>
+      <c r="D4" s="2">
+        <v>-0.78180000000000005</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.53659999999999997</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1.0477000000000001</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1.9388000000000001</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1.9984999999999999</v>
+      </c>
+      <c r="I4" s="2">
+        <v>1.948</v>
+      </c>
+      <c r="J4" s="2">
+        <v>2.8677999999999999</v>
+      </c>
+      <c r="K4" s="2">
+        <v>3.26</v>
+      </c>
+      <c r="L4" s="2">
+        <v>2.2513000000000001</v>
+      </c>
+      <c r="M4" s="2">
+        <v>1.9187000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" s="2" customFormat="1">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:24">
+      <c r="B5" s="2">
+        <v>1.5094000000000001</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.40570000000000001</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.59989999999999999</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1.2909999999999999</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1.5787</v>
+      </c>
+      <c r="G5" s="2">
+        <v>-0.50419999999999998</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1.659</v>
+      </c>
+      <c r="I5" s="2">
+        <v>1.728</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0.4889</v>
+      </c>
+      <c r="K5" s="2">
+        <v>-0.29909999999999998</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0.98629999999999995</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0.95779999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" s="2" customFormat="1">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:24">
+      <c r="B6" s="2">
+        <v>-0.41689999999999999</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.6492</v>
+      </c>
+      <c r="D6" s="2">
+        <v>-0.12590000000000001</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.71489999999999998</v>
+      </c>
+      <c r="F6" s="2">
+        <v>4.5699999999999998E-2</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.29320000000000002</v>
+      </c>
+      <c r="H6" s="2">
+        <v>-0.3901</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0.2321</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0.92379999999999995</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0.31740000000000002</v>
+      </c>
+      <c r="L6" s="2">
+        <v>-2.52E-2</v>
+      </c>
+      <c r="M6" s="2">
+        <v>1.0246</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" s="2" customFormat="1">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:24">
+      <c r="B7" s="2">
+        <v>0.41020000000000001</v>
+      </c>
+      <c r="C7" s="2">
+        <v>-0.92030000000000001</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.37859999999999999</v>
+      </c>
+      <c r="E7" s="2">
+        <v>-0.81689999999999996</v>
+      </c>
+      <c r="F7" s="2">
+        <v>3.0099999999999998E-2</v>
+      </c>
+      <c r="G7" s="2">
+        <v>-1.4461999999999999</v>
+      </c>
+      <c r="H7" s="2">
+        <v>-0.30249999999999999</v>
+      </c>
+      <c r="I7" s="2">
+        <v>-0.37269999999999998</v>
+      </c>
+      <c r="J7" s="2">
+        <v>-0.2195</v>
+      </c>
+      <c r="K7" s="2">
+        <v>-1.1638999999999999</v>
+      </c>
+      <c r="L7" s="2">
+        <v>0.26190000000000002</v>
+      </c>
+      <c r="M7" s="2">
+        <v>-0.52849999999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="2" customFormat="1">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:24">
+      <c r="B8" s="2">
+        <v>2.9630999999999998</v>
+      </c>
+      <c r="C8" s="2">
+        <v>5.4000000000000003E-3</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1.0226999999999999</v>
+      </c>
+      <c r="E8" s="2">
+        <v>-1.8079000000000001</v>
+      </c>
+      <c r="F8" s="2">
+        <v>2.6496</v>
+      </c>
+      <c r="G8" s="2">
+        <v>1.8896999999999999</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1.3274999999999999</v>
+      </c>
+      <c r="I8" s="2">
+        <v>-2.4363000000000001</v>
+      </c>
+      <c r="J8" s="2">
+        <v>1.3018000000000001</v>
+      </c>
+      <c r="K8" s="2">
+        <v>-0.26040000000000002</v>
+      </c>
+      <c r="L8" s="2">
+        <v>2.3205</v>
+      </c>
+      <c r="M8" s="2">
+        <v>-0.2676</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" s="2" customFormat="1">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:24">
+      <c r="B9" s="2">
+        <v>0.83460000000000001</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.54579999999999995</v>
+      </c>
+      <c r="D9" s="2">
+        <v>-0.40350000000000003</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.5827</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1.0075000000000001</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0.80379999999999996</v>
+      </c>
+      <c r="H9" s="2">
+        <v>1.1451</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0.6532</v>
+      </c>
+      <c r="J9" s="2">
+        <v>1.4213</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0.75490000000000002</v>
+      </c>
+      <c r="L9" s="2">
+        <v>0.33239999999999997</v>
+      </c>
+      <c r="M9" s="2">
+        <v>0.34039999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" s="2" customFormat="1">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:24">
+      <c r="B10" s="2">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.89349999999999996</v>
+      </c>
+      <c r="D10" s="2">
+        <v>3.44E-2</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.92530000000000001</v>
+      </c>
+      <c r="F10" s="2">
+        <v>-0.28220000000000001</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0.8125</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0.4466</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0.3866</v>
+      </c>
+      <c r="J10" s="2">
+        <v>-0.1762</v>
+      </c>
+      <c r="K10" s="2">
+        <v>0.49059999999999998</v>
+      </c>
+      <c r="L10" s="2">
+        <v>0.49409999999999998</v>
+      </c>
+      <c r="M10" s="2">
+        <v>0.45229999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" s="2" customFormat="1">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:24">
+      <c r="B11" s="2">
+        <v>-0.19409999999999999</v>
+      </c>
+      <c r="C11" s="2">
+        <v>-0.19769999999999999</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.32219999999999999</v>
+      </c>
+      <c r="E11" s="5">
+        <v>-2.3199999999999998E-2</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0.40579999999999999</v>
+      </c>
+      <c r="G11" s="2">
+        <v>-0.84</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0.4143</v>
+      </c>
+      <c r="I11" s="5">
+        <v>-6.6E-3</v>
+      </c>
+      <c r="J11" s="6">
+        <v>0.154</v>
+      </c>
+      <c r="K11" s="2">
+        <v>-0.1119</v>
+      </c>
+      <c r="L11" s="2">
+        <v>0.41210000000000002</v>
+      </c>
+      <c r="M11" s="2">
+        <v>0.16170000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" s="2" customFormat="1">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:24">
+      <c r="B12" s="2">
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.39439999999999997</v>
+      </c>
+      <c r="D12" s="2">
+        <v>-1.01E-2</v>
+      </c>
+      <c r="E12" s="2">
+        <v>-0.85629999999999995</v>
+      </c>
+      <c r="F12" s="2">
+        <v>-0.1573</v>
+      </c>
+      <c r="G12" s="2">
+        <v>-0.13389999999999999</v>
+      </c>
+      <c r="H12" s="2">
+        <v>-0.1171</v>
+      </c>
+      <c r="I12" s="5">
+        <v>-0.1361</v>
+      </c>
+      <c r="J12" s="2">
+        <v>0.3775</v>
+      </c>
+      <c r="K12" s="2">
+        <v>0.45390000000000003</v>
+      </c>
+      <c r="L12" s="2">
+        <v>0.33310000000000001</v>
+      </c>
+      <c r="M12" s="2">
+        <v>0.20960000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" s="2" customFormat="1">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:24">
+      <c r="B13" s="5">
+        <v>-3.9300000000000002E-2</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0.14910000000000001</v>
+      </c>
+      <c r="D13" s="2">
+        <v>-0.96150000000000002</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.69450000000000001</v>
+      </c>
+      <c r="F13" s="2">
+        <v>-1.177</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0.155</v>
+      </c>
+      <c r="H13" s="2">
+        <v>-1.3154999999999999</v>
+      </c>
+      <c r="I13" s="2">
+        <v>-0.11840000000000001</v>
+      </c>
+      <c r="J13" s="2">
+        <v>-1.0330999999999999</v>
+      </c>
+      <c r="K13" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L13" s="2">
+        <v>-0.74029999999999996</v>
+      </c>
+      <c r="M13" s="2">
+        <v>0.72799999999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" s="2" customFormat="1">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:24">
+      <c r="B14" s="2">
+        <v>-0.87780000000000002</v>
+      </c>
+      <c r="C14" s="2">
+        <v>-0.54210000000000003</v>
+      </c>
+      <c r="D14" s="2">
+        <v>-1.4449000000000001</v>
+      </c>
+      <c r="E14" s="2">
+        <v>-0.64190000000000003</v>
+      </c>
+      <c r="F14" s="2">
+        <v>-0.98599999999999999</v>
+      </c>
+      <c r="G14" s="2">
+        <v>-2.24E-2</v>
+      </c>
+      <c r="H14" s="2">
+        <v>-0.44590000000000002</v>
+      </c>
+      <c r="I14" s="2">
+        <v>-0.13830000000000001</v>
+      </c>
+      <c r="J14" s="2">
+        <v>0.93240000000000001</v>
+      </c>
+      <c r="K14" s="2">
+        <v>1.2888999999999999</v>
+      </c>
+      <c r="L14" s="2">
+        <v>0.65710000000000002</v>
+      </c>
+      <c r="M14" s="2">
+        <v>0.97740000000000005</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" s="2" customFormat="1">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:24">
+      <c r="B15" s="2">
+        <v>-1.7099</v>
+      </c>
+      <c r="C15" s="2">
+        <v>-1.3897999999999999</v>
+      </c>
+      <c r="D15" s="2">
+        <v>-2.1356000000000002</v>
+      </c>
+      <c r="E15" s="2">
+        <v>-1.6841999999999999</v>
+      </c>
+      <c r="F15" s="2">
+        <v>-0.12379999999999999</v>
+      </c>
+      <c r="G15" s="2">
+        <v>-1.0174000000000001</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0.37</v>
+      </c>
+      <c r="I15" s="2">
+        <v>-1.6722999999999999</v>
+      </c>
+      <c r="J15" s="2">
+        <v>-0.25900000000000001</v>
+      </c>
+      <c r="K15" s="2">
+        <v>-0.20080000000000001</v>
+      </c>
+      <c r="L15" s="2">
+        <v>-1.5284</v>
+      </c>
+      <c r="M15" s="2">
+        <v>-1.0412999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" s="2" customFormat="1">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:24">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+      <c r="B16" s="2">
+        <v>-1.903</v>
+      </c>
+      <c r="C16" s="5">
+        <v>-0.14449999999999999</v>
+      </c>
+      <c r="D16" s="2">
+        <v>1.5545</v>
+      </c>
+      <c r="E16" s="2">
+        <v>-8.4900000000000003E-2</v>
+      </c>
+      <c r="F16" s="2">
+        <v>-0.61270000000000002</v>
+      </c>
+      <c r="G16" s="2">
+        <v>1.2343</v>
+      </c>
+      <c r="H16" s="2">
+        <v>-0.58879999999999999</v>
+      </c>
+      <c r="I16" s="2">
+        <v>-0.87460000000000004</v>
+      </c>
+      <c r="J16" s="2">
+        <v>-0.88219999999999998</v>
+      </c>
+      <c r="K16" s="2">
+        <v>0.6754</v>
+      </c>
+      <c r="L16" s="2">
+        <v>-0.73409999999999997</v>
+      </c>
+      <c r="M16" s="2">
+        <v>-0.5958</v>
+      </c>
+    </row>
+    <row r="17" spans="7:7" s="2" customFormat="1">
       <c r="G17" s="3"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
-      <c r="Q17" s="2"/>
-      <c r="R17" s="2"/>
-      <c r="S17" s="2"/>
-      <c r="T17" s="2"/>
-      <c r="U17" s="2"/>
-      <c r="V17" s="2"/>
-      <c r="W17" s="2"/>
-      <c r="X17" s="2"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:X1">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(B1))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -2556,9 +2764,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="16384" width="10.83203125" style="2"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="2" t="s">
@@ -3376,10 +3587,13 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="16384" width="10.83203125" style="2"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="2" t="s">
@@ -4194,13 +4408,186 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="21.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="7">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="7">
+        <v>100000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="7">
+        <v>9.9999999999999995E-7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="7">
+        <v>100000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="7">
+        <v>9.9999999999999995E-7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="8">
+        <v>15</v>
+      </c>
+      <c r="C13" s="2">
+        <v>30</v>
+      </c>
+      <c r="D13" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0</v>
+      </c>
+      <c r="C15" s="2">
+        <v>5</v>
+      </c>
+      <c r="D15" s="2">
+        <v>10</v>
+      </c>
+      <c r="E15" s="2">
+        <v>15</v>
+      </c>
+      <c r="F15" s="2">
+        <v>20</v>
+      </c>
+      <c r="G15" s="2">
+        <v>25</v>
+      </c>
+      <c r="H15" s="2">
+        <v>30</v>
+      </c>
+      <c r="I15" s="2">
+        <v>35</v>
+      </c>
+      <c r="J15" s="2">
+        <v>40</v>
+      </c>
+      <c r="K15" s="2">
+        <v>45</v>
+      </c>
+      <c r="L15" s="2">
+        <v>50</v>
+      </c>
+      <c r="M15" s="2">
+        <v>55</v>
+      </c>
+      <c r="N15" s="2">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4214,16 +4601,19 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="16384" width="10.83203125" style="2"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -4231,7 +4621,7 @@
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>0</v>
       </c>
     </row>
@@ -4239,7 +4629,7 @@
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>0</v>
       </c>
     </row>
@@ -4247,7 +4637,7 @@
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>0</v>
       </c>
     </row>
@@ -4255,7 +4645,7 @@
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>0</v>
       </c>
     </row>
@@ -4263,7 +4653,7 @@
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>0</v>
       </c>
     </row>
@@ -4271,7 +4661,7 @@
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>0</v>
       </c>
     </row>
@@ -4279,7 +4669,7 @@
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>0</v>
       </c>
     </row>
@@ -4287,7 +4677,7 @@
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
         <v>0</v>
       </c>
     </row>
@@ -4295,7 +4685,7 @@
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="2">
         <v>0</v>
       </c>
     </row>
@@ -4303,7 +4693,7 @@
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="2">
         <v>0</v>
       </c>
     </row>
@@ -4311,7 +4701,7 @@
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="2">
         <v>0</v>
       </c>
     </row>
@@ -4319,7 +4709,7 @@
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="2">
         <v>0</v>
       </c>
     </row>
@@ -4327,7 +4717,7 @@
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="2">
         <v>0</v>
       </c>
     </row>
@@ -4335,7 +4725,7 @@
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="2">
         <v>0</v>
       </c>
     </row>
@@ -4343,12 +4733,13 @@
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="2">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
completed dHAP4 input sheet
</commit_message>
<xml_diff>
--- a/data/GRNmap_input_workbooks/15-genes_28-edges_BK-dHAP4-fam_no-strains-added_Sigmoid_estimation.xlsx
+++ b/data/GRNmap_input_workbooks/15-genes_28-edges_BK-dHAP4-fam_no-strains-added_Sigmoid_estimation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="0" windowWidth="23140" windowHeight="15540" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="3300" yWindow="0" windowWidth="25120" windowHeight="15040" tabRatio="500" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="production_rates" sheetId="5" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="40">
   <si>
     <t>ACE2</t>
   </si>
@@ -141,6 +141,12 @@
   <si>
     <t>dhap4</t>
   </si>
+  <si>
+    <t>optimization_parameter</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
 </sst>
 </file>
 
@@ -206,7 +212,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="235">
+  <cellStyleXfs count="237">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -442,8 +448,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -451,10 +459,12 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="235">
+  <cellStyles count="237">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -572,6 +582,7 @@
     <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -689,30 +700,10 @@
     <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
@@ -1349,7 +1340,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:N2"/>
     </sheetView>
   </sheetViews>
@@ -1358,7 +1349,7 @@
     <col min="1" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1">
+    <row r="1" spans="1:14">
       <c r="A1" s="2" t="s">
         <v>16</v>
       </c>
@@ -1402,7 +1393,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="2" customFormat="1">
+    <row r="2" spans="1:14">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1446,7 +1437,7 @@
         <v>-1.2497</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="2" customFormat="1">
+    <row r="3" spans="1:14">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1490,7 +1481,7 @@
         <v>-0.92479999999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="2" customFormat="1">
+    <row r="4" spans="1:14">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -1534,7 +1525,7 @@
         <v>1.4784999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="2" customFormat="1">
+    <row r="5" spans="1:14">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -1578,7 +1569,7 @@
         <v>-0.35849999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="2" customFormat="1">
+    <row r="6" spans="1:14">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -1622,7 +1613,7 @@
         <v>0.1953</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="2" customFormat="1">
+    <row r="7" spans="1:14">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -1666,7 +1657,7 @@
         <v>-1.8463000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="2" customFormat="1">
+    <row r="8" spans="1:14">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -1710,7 +1701,7 @@
         <v>2.2172000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:14" s="2" customFormat="1">
+    <row r="9" spans="1:14">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -1754,7 +1745,7 @@
         <v>-0.12709999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:14" s="2" customFormat="1">
+    <row r="10" spans="1:14">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -1798,7 +1789,7 @@
         <v>-1.0367</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="2" customFormat="1">
+    <row r="11" spans="1:14">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -1842,7 +1833,7 @@
         <v>-0.27479999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="2" customFormat="1">
+    <row r="12" spans="1:14">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -1886,7 +1877,7 @@
         <v>0.28120000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:14" s="2" customFormat="1">
+    <row r="13" spans="1:14">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -1930,7 +1921,7 @@
         <v>9.7000000000000003E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" s="2" customFormat="1">
+    <row r="14" spans="1:14">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -1974,7 +1965,7 @@
         <v>-0.72499999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:14" s="2" customFormat="1">
+    <row r="15" spans="1:14">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -2018,7 +2009,7 @@
         <v>-0.51170000000000004</v>
       </c>
     </row>
-    <row r="16" spans="1:14" s="2" customFormat="1">
+    <row r="16" spans="1:14">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -2062,7 +2053,7 @@
         <v>2.6345999999999998</v>
       </c>
     </row>
-    <row r="17" spans="7:7" s="2" customFormat="1">
+    <row r="17" spans="7:7">
       <c r="G17" s="3"/>
     </row>
   </sheetData>
@@ -2089,7 +2080,7 @@
     <col min="1" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1">
+    <row r="1" spans="1:14">
       <c r="A1" s="2" t="s">
         <v>16</v>
       </c>
@@ -2131,7 +2122,7 @@
       </c>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:14" s="2" customFormat="1">
+    <row r="2" spans="1:14">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2172,7 +2163,7 @@
         <v>0.19850000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="2" customFormat="1">
+    <row r="3" spans="1:14">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -2213,7 +2204,7 @@
         <v>-1.5982000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="2" customFormat="1">
+    <row r="4" spans="1:14">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -2254,7 +2245,7 @@
         <v>1.9187000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="2" customFormat="1">
+    <row r="5" spans="1:14">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -2295,7 +2286,7 @@
         <v>0.95779999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="2" customFormat="1">
+    <row r="6" spans="1:14">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -2336,7 +2327,7 @@
         <v>1.0246</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="2" customFormat="1">
+    <row r="7" spans="1:14">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -2377,7 +2368,7 @@
         <v>-0.52849999999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="2" customFormat="1">
+    <row r="8" spans="1:14">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -2418,7 +2409,7 @@
         <v>-0.2676</v>
       </c>
     </row>
-    <row r="9" spans="1:14" s="2" customFormat="1">
+    <row r="9" spans="1:14">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -2459,7 +2450,7 @@
         <v>0.34039999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:14" s="2" customFormat="1">
+    <row r="10" spans="1:14">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -2500,7 +2491,7 @@
         <v>0.45229999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="2" customFormat="1">
+    <row r="11" spans="1:14">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -2541,7 +2532,7 @@
         <v>0.16170000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="2" customFormat="1">
+    <row r="12" spans="1:14">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -2582,7 +2573,7 @@
         <v>0.20960000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:14" s="2" customFormat="1">
+    <row r="13" spans="1:14">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -2623,7 +2614,7 @@
         <v>0.72799999999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:14" s="2" customFormat="1">
+    <row r="14" spans="1:14">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -2664,7 +2655,7 @@
         <v>0.97740000000000005</v>
       </c>
     </row>
-    <row r="15" spans="1:14" s="2" customFormat="1">
+    <row r="15" spans="1:14">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -2705,7 +2696,7 @@
         <v>-1.0412999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:14" s="2" customFormat="1">
+    <row r="16" spans="1:14">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -2746,7 +2737,7 @@
         <v>-0.5958</v>
       </c>
     </row>
-    <row r="17" spans="7:7" s="2" customFormat="1">
+    <row r="17" spans="7:7">
       <c r="G17" s="3"/>
     </row>
   </sheetData>
@@ -4408,10 +4399,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -4422,166 +4413,174 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="7">
-        <v>2E-3</v>
+        <v>38</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="5">
-        <v>1</v>
+        <v>20</v>
+      </c>
+      <c r="B2" s="9">
+        <v>2E-3</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="7">
-        <v>100000000</v>
+        <v>21</v>
+      </c>
+      <c r="B3" s="8">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="7">
-        <v>9.9999999999999995E-7</v>
+        <v>22</v>
+      </c>
+      <c r="B4" s="9">
+        <v>100000000</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="7">
-        <v>100000000</v>
+        <v>23</v>
+      </c>
+      <c r="B5" s="9">
+        <v>9.9999999999999995E-7</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="7">
-        <v>9.9999999999999995E-7</v>
+        <v>24</v>
+      </c>
+      <c r="B6" s="9">
+        <v>100000000</v>
       </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>35</v>
+        <v>25</v>
+      </c>
+      <c r="B7" s="9">
+        <v>9.9999999999999995E-7</v>
       </c>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="8">
-        <v>0</v>
+        <v>26</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="8">
-        <v>1</v>
+        <v>27</v>
+      </c>
+      <c r="B9" s="10">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="8">
+        <v>28</v>
+      </c>
+      <c r="B10" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="8">
-        <v>0</v>
+        <v>29</v>
+      </c>
+      <c r="B11" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="8">
+        <v>30</v>
+      </c>
+      <c r="B12" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="8">
-        <v>15</v>
-      </c>
-      <c r="C13" s="2">
-        <v>30</v>
-      </c>
-      <c r="D13" s="2">
-        <v>60</v>
+        <v>31</v>
+      </c>
+      <c r="B13" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
+      </c>
+      <c r="B14" s="7">
+        <v>15</v>
+      </c>
+      <c r="C14" s="2">
+        <v>30</v>
+      </c>
+      <c r="D14" s="2">
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="2">
-        <v>0</v>
-      </c>
-      <c r="C15" s="2">
+      <c r="B16" s="2">
+        <v>0</v>
+      </c>
+      <c r="C16" s="2">
         <v>5</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D16" s="2">
         <v>10</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E16" s="2">
         <v>15</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F16" s="2">
         <v>20</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G16" s="2">
         <v>25</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H16" s="2">
         <v>30</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I16" s="2">
         <v>35</v>
       </c>
-      <c r="J15" s="2">
+      <c r="J16" s="2">
         <v>40</v>
       </c>
-      <c r="K15" s="2">
+      <c r="K16" s="2">
         <v>45</v>
       </c>
-      <c r="L15" s="2">
+      <c r="L16" s="2">
         <v>50</v>
       </c>
-      <c r="M15" s="2">
+      <c r="M16" s="2">
         <v>55</v>
       </c>
-      <c r="N15" s="2">
+      <c r="N16" s="2">
         <v>60</v>
       </c>
     </row>

</xml_diff>